<commit_message>
Add deactivate users task
git-tfs-id: [https://hayessoftware.visualstudio.com/]$/Hayes Integration;C9250
</commit_message>
<xml_diff>
--- a/DEV/LDAP_UserProcess/LDAP_UserProcess/Template.xlsx
+++ b/DEV/LDAP_UserProcess/LDAP_UserProcess/Template.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nblakely\Desktop\Northside\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\VSO\Hayes Integrations\DEV\LDAP_UserProcess\LDAP_UserProcess\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="146" uniqueCount="111">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="147" uniqueCount="112">
   <si>
     <t>PURCHASE_VIEW</t>
   </si>
@@ -359,6 +359,9 @@
   </si>
   <si>
     <t>Site View users will have Permissions updated - only those permissions in the file will be retained</t>
+  </si>
+  <si>
+    <t>All current users will be deactivated</t>
   </si>
 </sst>
 </file>
@@ -508,6 +511,23 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -543,6 +563,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -695,10 +732,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:C27"/>
+  <dimension ref="A2:C28"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I10" sqref="I10"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="B25" sqref="B25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -808,21 +845,26 @@
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B24" s="3" t="s">
-        <v>107</v>
+        <v>111</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B25" s="3" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B26" s="3" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B27" s="3" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B28" s="3" t="s">
         <v>110</v>
       </c>
     </row>

</xml_diff>